<commit_message>
docs: se agregan documentos del 5 trimestre
</commit_message>
<xml_diff>
--- a/5.Pruebas/Matriz Trazabilidad/MatrizTrazabilidad.xlsx
+++ b/5.Pruebas/Matriz Trazabilidad/MatrizTrazabilidad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\F\Desktop\QrLean\5.Pruebas\Matriz Trazabilidad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{618E6101-E94C-44C8-9BA4-3D5EAD5F142A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BF8E8EF-C26E-48B8-870B-1A1DC52507FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{DDDD71EA-B3F4-4B94-BA38-70AE9AAB84CC}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="50">
   <si>
     <t>Id Req</t>
   </si>
@@ -75,9 +75,6 @@
     <t>Req funcional</t>
   </si>
   <si>
-    <t>Incompleto</t>
-  </si>
-  <si>
     <t>Al intentar acceder a cualquier parte del aplicativo exceptuando paginas iniciales de explicación la aplicación requerirá iniciar sesión con identificación, tipo de identificación y contraseña, y así dar acceso a la plataforma, y así mismo poder cerrar su sesión cuando no requiera acceder más al sistema siendo redirigido al inicio del aplicativo.</t>
   </si>
   <si>
@@ -178,6 +175,12 @@
   </si>
   <si>
     <t>El sistema permitirá desde el dashboard con el rol de aprendiz:-la creación de una solicitud de cambio de asistencia, ingresando los siguientes datos:Asunto, contenido, instructor, evidencia.-la visualización de todas las solicitudes de cambio de asistencia hechas por el aprendiz.-cerrar/cancelar una solicitud de cambio de asistencia.</t>
+  </si>
+  <si>
+    <t>En curso</t>
+  </si>
+  <si>
+    <t>Codigo fuente</t>
   </si>
 </sst>
 </file>
@@ -569,7 +572,7 @@
   <dimension ref="B2:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="J4" sqref="J4:J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -581,14 +584,14 @@
     <col min="7" max="7" width="31" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="25.85546875" customWidth="1"/>
     <col min="9" max="9" width="20" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="23" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="45" x14ac:dyDescent="0.25">
       <c r="K2" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
@@ -640,33 +643,33 @@
         <v>4</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="G4" s="2">
         <v>44538</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I4">
         <v>2</v>
       </c>
       <c r="J4" t="s">
+        <v>49</v>
+      </c>
+      <c r="K4" t="s">
         <v>16</v>
       </c>
-      <c r="K4" t="s">
-        <v>17</v>
-      </c>
       <c r="L4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="2:12" ht="94.5" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="D5" t="s">
         <v>13</v>
@@ -675,33 +678,33 @@
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="G5" s="2">
         <v>44539</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I5">
         <v>2</v>
       </c>
       <c r="J5" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
       <c r="K5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="375" x14ac:dyDescent="0.25">
       <c r="B6" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>24</v>
       </c>
       <c r="D6" t="s">
         <v>13</v>
@@ -709,31 +712,34 @@
       <c r="E6">
         <v>4</v>
       </c>
+      <c r="F6" t="s">
+        <v>48</v>
+      </c>
       <c r="G6" s="2">
         <v>44540</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I6">
         <v>4</v>
       </c>
       <c r="J6" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="2:12" ht="360" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>28</v>
       </c>
       <c r="D7" t="s">
         <v>13</v>
@@ -742,33 +748,33 @@
         <v>3</v>
       </c>
       <c r="F7" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="G7" s="2">
         <v>44541</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I7">
         <v>4</v>
       </c>
       <c r="J7" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="2:12" ht="375" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>32</v>
       </c>
       <c r="D8" t="s">
         <v>13</v>
@@ -777,33 +783,33 @@
         <v>3</v>
       </c>
       <c r="F8" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="G8" s="2">
         <v>44542</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I8">
         <v>4</v>
       </c>
       <c r="J8" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
       <c r="K8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="2:12" ht="240" x14ac:dyDescent="0.25">
       <c r="B9" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>35</v>
       </c>
       <c r="D9" t="s">
         <v>13</v>
@@ -812,33 +818,33 @@
         <v>3</v>
       </c>
       <c r="F9" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="G9" s="2">
         <v>44543</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I9">
         <v>4</v>
       </c>
       <c r="J9" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
       <c r="K9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="2:12" ht="150" x14ac:dyDescent="0.25">
       <c r="B10" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>38</v>
       </c>
       <c r="D10" t="s">
         <v>13</v>
@@ -847,33 +853,33 @@
         <v>2</v>
       </c>
       <c r="F10" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="G10" s="2">
         <v>44544</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I10">
         <v>2</v>
       </c>
       <c r="J10" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
       <c r="K10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="2:12" ht="150" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>41</v>
       </c>
       <c r="D11" t="s">
         <v>13</v>
@@ -882,33 +888,33 @@
         <v>2</v>
       </c>
       <c r="F11" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="G11" s="2">
         <v>44545</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I11">
         <v>2</v>
       </c>
       <c r="J11" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
       <c r="K11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="2:12" ht="75" x14ac:dyDescent="0.25">
       <c r="B12" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D12" t="s">
         <v>13</v>
@@ -917,33 +923,33 @@
         <v>2</v>
       </c>
       <c r="F12" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="G12" s="2">
         <v>44546</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I12">
         <v>4</v>
       </c>
       <c r="J12" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
       <c r="K12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="2:12" ht="211.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D13" t="s">
         <v>13</v>
@@ -952,25 +958,25 @@
         <v>2</v>
       </c>
       <c r="F13" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="G13" s="2">
         <v>44547</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I13">
         <v>2</v>
       </c>
       <c r="J13" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
       <c r="K13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>